<commit_message>
Fixed some fund fees
</commit_message>
<xml_diff>
--- a/presentations/Tabla Fondos.xlsx
+++ b/presentations/Tabla Fondos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresp/Documents/R Projects/Trading bloque/presentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50D7AA4-1A7C-234F-B575-9603C402225F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ADF9BF-B9F1-9A4A-A16E-B73EF70FC6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="2520" yWindow="2960" windowWidth="25740" windowHeight="14520" xr2:uid="{721C987A-A8B3-1944-995A-C5D6A9D99DFD}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="2380" yWindow="10160" windowWidth="25740" windowHeight="14520" xr2:uid="{721C987A-A8B3-1944-995A-C5D6A9D99DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,21 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Funds</t>
-  </si>
-  <si>
-    <t>AUM in Millions</t>
-  </si>
-  <si>
-    <t>Management  Fee</t>
-  </si>
-  <si>
-    <t>Performance Fee</t>
-  </si>
-  <si>
-    <t>Inception Year</t>
-  </si>
-  <si>
     <t>Dunn</t>
   </si>
   <si>
@@ -69,6 +54,21 @@
   </si>
   <si>
     <t>Transtrend</t>
+  </si>
+  <si>
+    <t>Fund</t>
+  </si>
+  <si>
+    <t>AUM</t>
+  </si>
+  <si>
+    <t>M_Fee</t>
+  </si>
+  <si>
+    <t>P_Fee</t>
+  </si>
+  <si>
+    <t>Starting_Year</t>
   </si>
 </sst>
 </file>
@@ -84,15 +84,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -180,37 +181,37 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -530,127 +531,127 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="101" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
         <v>663</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0.25</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1984</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
         <v>170</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>0.01</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>0.2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>1988</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="9">
-        <v>69</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>222</v>
+      </c>
+      <c r="C4" s="9">
         <v>0.02</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>0.2</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>1999</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6">
-        <v>504</v>
-      </c>
-      <c r="C5" s="7">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C5" s="6">
         <v>0.01</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>2014</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="9">
+      <c r="A6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8">
         <v>6361</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>0.01</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>0.2</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>2004</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
         <v>4582</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>0.2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>1995</v>
       </c>
     </row>

</xml_diff>